<commit_message>
fixed number of springs
</commit_message>
<xml_diff>
--- a/specifications/Price.xlsx
+++ b/specifications/Price.xlsx
@@ -44,9 +44,6 @@
     <t>Bolt/Screw</t>
   </si>
   <si>
-    <t>Spring</t>
-  </si>
-  <si>
     <t>94125K542</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Springx2</t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -133,7 +133,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -418,7 +418,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -455,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <f>E2/F2</f>
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D4" si="0">E3/F3</f>
@@ -488,14 +488,14 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>2.0720000000000001</v>
+        <f>(E4/F4)*2</f>
+        <v>4.1440000000000001</v>
       </c>
       <c r="E4" s="1">
         <v>10.36</v>
@@ -506,34 +506,34 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
         <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>23.88</v>
@@ -546,12 +546,12 @@
         <v>48</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>9.2200000000000006</v>
@@ -564,12 +564,12 @@
         <v>48</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>0.88</v>
@@ -582,16 +582,16 @@
         <v>48</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <f>SUM(D2:D11)</f>
-        <v>3.8383400000000001</v>
+        <v>5.9103399999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>